<commit_message>
Refactoring and preparations for downloading datasets metadata masterfiles.
</commit_message>
<xml_diff>
--- a/src/main/resources/spreadsheets/datasets.xlsx
+++ b/src/main/resources/spreadsheets/datasets.xlsx
@@ -7,14 +7,15 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="METADATA" sheetId="1" r:id="rId1"/>
+    <sheet name="CONFIGURATION" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
   <si>
     <t>DESCRIPTION</t>
   </si>
@@ -25,9 +26,6 @@
     <t>DATE_ISSUED</t>
   </si>
   <si>
-    <t>2016-05-01T00:00:00Z</t>
-  </si>
-  <si>
     <t>LICENSE_URI</t>
   </si>
   <si>
@@ -37,52 +35,76 @@
     <t>PERIODICITY_URI</t>
   </si>
   <si>
-    <t>http://www.neti.ee</t>
-  </si>
-  <si>
-    <t>http://www.license.ee</t>
-  </si>
-  <si>
-    <t>http://www.status.ee</t>
-  </si>
-  <si>
-    <t>http://www.periodicity.ee</t>
-  </si>
-  <si>
     <t>KEYWORD</t>
   </si>
   <si>
-    <t>word1</t>
-  </si>
-  <si>
-    <t>word2</t>
-  </si>
-  <si>
-    <t>word3</t>
-  </si>
-  <si>
-    <t>word4</t>
-  </si>
-  <si>
-    <t>word5</t>
-  </si>
-  <si>
-    <t>andmehulk56</t>
-  </si>
-  <si>
-    <t>andmehulk56 title</t>
-  </si>
-  <si>
-    <t>andmehulk56 description</t>
-  </si>
-  <si>
-    <t>word6</t>
-  </si>
-  <si>
     <t>IDENTIFIER</t>
   </si>
   <si>
     <t>TITLE</t>
+  </si>
+  <si>
+    <t>COLUMN_TITLE</t>
+  </si>
+  <si>
+    <t>RDF_PROPERTY_URI</t>
+  </si>
+  <si>
+    <t>http://purl.org/dc/terms/identifier</t>
+  </si>
+  <si>
+    <t>http://purl.org/dc/terms/title</t>
+  </si>
+  <si>
+    <t>http://purl.org/dc/terms/description</t>
+  </si>
+  <si>
+    <t>http://purl.org/dc/terms/issued</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/ns/dcat#keyword</t>
+  </si>
+  <si>
+    <t>http://purl.org/linked-data/cube#structure</t>
+  </si>
+  <si>
+    <t>http://purl.org/dc/terms/license</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/ns/adms#status</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/ns/dcat#accrualPeriodicity</t>
+  </si>
+  <si>
+    <t>RDF_TEMPLATE_VARIABLE</t>
+  </si>
+  <si>
+    <t>DATASET_IDENTIFIER</t>
+  </si>
+  <si>
+    <t>DATASET_TITLE</t>
+  </si>
+  <si>
+    <t>DATASET_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>DATASET_ISSUED</t>
+  </si>
+  <si>
+    <t>DATASET_KEYWORD</t>
+  </si>
+  <si>
+    <t>DATASET_DSD</t>
+  </si>
+  <si>
+    <t>DATASET_LICENSE</t>
+  </si>
+  <si>
+    <t>DATASET_STATUS</t>
+  </si>
+  <si>
+    <t>DATASET_PERIODICITY</t>
   </si>
 </sst>
 </file>
@@ -123,7 +145,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -140,15 +162,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -456,9 +491,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -475,10 +508,10 @@
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -487,222 +520,200 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.5703125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="74.5703125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>10</v>
+      <c r="C10" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
-    <hyperlink ref="G2" r:id="rId2"/>
-    <hyperlink ref="H2" r:id="rId3"/>
-    <hyperlink ref="I2" r:id="rId4"/>
-    <hyperlink ref="F3" r:id="rId5"/>
-    <hyperlink ref="F4" r:id="rId6"/>
-    <hyperlink ref="F5" r:id="rId7"/>
-    <hyperlink ref="F6" r:id="rId8"/>
-    <hyperlink ref="G3" r:id="rId9"/>
-    <hyperlink ref="G4" r:id="rId10"/>
-    <hyperlink ref="G5" r:id="rId11"/>
-    <hyperlink ref="G6" r:id="rId12"/>
-    <hyperlink ref="H3" r:id="rId13"/>
-    <hyperlink ref="H4" r:id="rId14"/>
-    <hyperlink ref="H5" r:id="rId15"/>
-    <hyperlink ref="H6" r:id="rId16"/>
-    <hyperlink ref="I3" r:id="rId17"/>
-    <hyperlink ref="I4" r:id="rId18"/>
-    <hyperlink ref="I5" r:id="rId19"/>
-    <hyperlink ref="I6" r:id="rId20"/>
-    <hyperlink ref="F7" r:id="rId21"/>
-    <hyperlink ref="G7" r:id="rId22"/>
-    <hyperlink ref="H7" r:id="rId23"/>
-    <hyperlink ref="I7" r:id="rId24"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B5" r:id="rId4"/>
+    <hyperlink ref="B6" r:id="rId5" location="keyword"/>
+    <hyperlink ref="B7" r:id="rId6" location="structure"/>
+    <hyperlink ref="B8" r:id="rId7"/>
+    <hyperlink ref="B9" r:id="rId8" location="status"/>
+    <hyperlink ref="B10" r:id="rId9" location="accrualPeriodicity"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ODP upload rewrite + datasets export + lots of refactoring.
</commit_message>
<xml_diff>
--- a/src/main/resources/spreadsheets/datasets.xlsx
+++ b/src/main/resources/spreadsheets/datasets.xlsx
@@ -77,34 +77,34 @@
     <t>http://www.w3.org/ns/dcat#accrualPeriodicity</t>
   </si>
   <si>
-    <t>RDF_TEMPLATE_VARIABLE</t>
-  </si>
-  <si>
-    <t>DATASET_IDENTIFIER</t>
-  </si>
-  <si>
-    <t>DATASET_TITLE</t>
-  </si>
-  <si>
-    <t>DATASET_DESCRIPTION</t>
-  </si>
-  <si>
-    <t>DATASET_ISSUED</t>
-  </si>
-  <si>
-    <t>DATASET_KEYWORD</t>
-  </si>
-  <si>
-    <t>DATASET_DSD</t>
-  </si>
-  <si>
-    <t>DATASET_LICENSE</t>
-  </si>
-  <si>
-    <t>DATASET_STATUS</t>
-  </si>
-  <si>
-    <t>DATASET_PERIODICITY</t>
+    <t>BEAN_PROPERTY</t>
+  </si>
+  <si>
+    <t>identifier</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>issuedDateTimeStr</t>
+  </si>
+  <si>
+    <t>keyword</t>
+  </si>
+  <si>
+    <t>dsdUri</t>
+  </si>
+  <si>
+    <t>licenseUri</t>
+  </si>
+  <si>
+    <t>statusUri</t>
+  </si>
+  <si>
+    <t>periodicityUri</t>
   </si>
 </sst>
 </file>
@@ -491,7 +491,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -581,7 +583,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Preparations for specifying dataset catalogs in uploaded spreadsheets + Bugfix: completely empty rows in Excel were handled properly.
</commit_message>
<xml_diff>
--- a/src/main/resources/spreadsheets/datasets.xlsx
+++ b/src/main/resources/spreadsheets/datasets.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="METADATA" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
   <si>
     <t>DESCRIPTION</t>
   </si>
@@ -105,6 +105,12 @@
   </si>
   <si>
     <t>periodicityUri</t>
+  </si>
+  <si>
+    <t>CATALOG_IDENTIFIER</t>
+  </si>
+  <si>
+    <t>catalogIdentifier</t>
   </si>
 </sst>
 </file>
@@ -489,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,13 +508,14 @@
     <col min="3" max="3" width="26.5703125" customWidth="1"/>
     <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.85546875" customWidth="1"/>
-    <col min="6" max="6" width="49" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="49" customWidth="1"/>
+    <col min="8" max="8" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -525,53 +532,56 @@
         <v>6</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F2" s="2"/>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F3" s="2"/>
+      <c r="J2" s="2"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F4" s="2"/>
+      <c r="J3" s="2"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F5" s="2"/>
+      <c r="J4" s="2"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F6" s="2"/>
+      <c r="J5" s="2"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F7" s="2"/>
+      <c r="J6" s="2"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -580,10 +590,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -701,6 +711,14 @@
       </c>
       <c r="C10" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dataset catalogs now also exported into the datasets spreadsheet.
</commit_message>
<xml_diff>
--- a/src/main/resources/spreadsheets/datasets.xlsx
+++ b/src/main/resources/spreadsheets/datasets.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
   <si>
     <t>DESCRIPTION</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>catalogIdentifier</t>
+  </si>
+  <si>
+    <t>dummy:catalogIdentifier</t>
   </si>
 </sst>
 </file>
@@ -593,7 +596,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -717,6 +720,9 @@
       <c r="A11" s="5" t="s">
         <v>30</v>
       </c>
+      <c r="B11" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="C11" t="s">
         <v>31</v>
       </c>
@@ -732,8 +738,9 @@
     <hyperlink ref="B8" r:id="rId7"/>
     <hyperlink ref="B9" r:id="rId8" location="status"/>
     <hyperlink ref="B10" r:id="rId9" location="accrualPeriodicity"/>
+    <hyperlink ref="B11" r:id="rId10" display="http://purl.org/dc/terms/license"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId10"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>